<commit_message>
update system to handle piecewise function input from excel file structure.
</commit_message>
<xml_diff>
--- a/models/test_structures/sysconfig_simple_linear.xlsx
+++ b/models/test_structures/sysconfig_simple_linear.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="106">
   <si>
     <t>Capacity by Generator (in MW)</t>
   </si>
@@ -177,19 +177,10 @@
     <t>damage_function</t>
   </si>
   <si>
-    <t>mode</t>
-  </si>
-  <si>
     <t>SYSTEM OUTPUT</t>
   </si>
   <si>
     <t>minimum</t>
-  </si>
-  <si>
-    <t>sigma_1</t>
-  </si>
-  <si>
-    <t>sigma_2</t>
   </si>
   <si>
     <t>NA</t>
@@ -333,6 +324,27 @@
   </si>
   <si>
     <t>beta</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>is_piecewise</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>upper_limit</t>
+  </si>
+  <si>
+    <t>lower_limit</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Not Available.</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1105,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1234,18 +1246,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1267,9 +1267,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1282,9 +1279,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1297,9 +1291,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1352,6 +1343,12 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="534">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2237,76 +2234,76 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="87" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="80" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="80" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="87" t="s">
-        <v>63</v>
+      <c r="C6" s="80" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2360,13 +2357,13 @@
     </row>
     <row r="2" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="41">
         <v>0</v>
@@ -2375,7 +2372,7 @@
         <v>45</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G2" s="43">
         <v>1</v>
@@ -2383,13 +2380,13 @@
     </row>
     <row r="3" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="41">
         <v>0.6</v>
@@ -2398,7 +2395,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G3" s="43">
         <v>1</v>
@@ -2406,13 +2403,13 @@
     </row>
     <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" s="41">
         <v>0.4</v>
@@ -2421,7 +2418,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G4" s="43">
         <v>1</v>
@@ -2435,16 +2432,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="41">
         <v>0</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="66" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G5" s="43">
         <v>1</v>
@@ -2501,24 +2498,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" s="47">
         <v>1</v>
@@ -2529,10 +2526,10 @@
     </row>
     <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C3" s="47">
         <v>1</v>
@@ -2543,7 +2540,7 @@
     </row>
     <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>15</v>
@@ -2583,21 +2580,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="30">
         <v>100</v>
@@ -2662,19 +2659,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2682,7 +2679,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C2" s="36">
         <v>250</v>
@@ -2712,1213 +2709,1312 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF804000"/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" customWidth="1"/>
-    <col min="5" max="6" width="14.125" style="2" customWidth="1"/>
-    <col min="7" max="11" width="11.125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="16.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="65.625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="44.625" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="3"/>
+    <col min="1" max="1" width="10.875" style="81"/>
+    <col min="2" max="2" width="22.625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="14.125" style="2" customWidth="1"/>
+    <col min="8" max="12" width="11.125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="2" customWidth="1"/>
+    <col min="15" max="15" width="16.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="65.625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="44.625" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="70" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="82">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="57" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="55" t="s">
+      <c r="E2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="19">
+        <v>0.42</v>
+      </c>
+      <c r="G2" s="19">
+        <v>0.375</v>
+      </c>
+      <c r="H2" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="20">
+        <v>1</v>
+      </c>
+      <c r="J2" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="56" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="77" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="K2" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="N2" s="20">
+        <f t="shared" ref="N2:N13" si="0">O2/NORMINV(0.95,0,1)</f>
+        <v>0.30397841595588471</v>
+      </c>
+      <c r="O2" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="82">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="50">
-        <v>1</v>
-      </c>
-      <c r="E2" s="19">
-        <v>0.42</v>
-      </c>
-      <c r="F2" s="19">
+      <c r="F3" s="21">
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="G3" s="21">
         <v>0.375</v>
       </c>
-      <c r="G2" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="H2" s="20">
-        <v>1</v>
-      </c>
-      <c r="I2" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" s="4">
-        <v>1</v>
-      </c>
-      <c r="M2" s="20">
-        <f t="shared" ref="M2:M13" si="0">N2/NORMINV(0.95,0,1)</f>
-        <v>0.30397841595588471</v>
-      </c>
-      <c r="N2" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="49">
-        <v>1</v>
-      </c>
-      <c r="E3" s="21">
-        <v>0.57000000000000006</v>
-      </c>
-      <c r="F3" s="21">
-        <v>0.375</v>
-      </c>
-      <c r="G3" s="22">
+      <c r="H3" s="22">
         <v>0.3</v>
       </c>
-      <c r="H3" s="22">
+      <c r="I3" s="22">
         <v>0</v>
       </c>
-      <c r="I3" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="6">
+      <c r="J3" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="6">
         <v>3</v>
       </c>
-      <c r="M3" s="22">
+      <c r="N3" s="22">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="N3" s="79">
-        <v>1</v>
-      </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="72">
+        <v>1</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>80</v>
+    <row r="4" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="82">
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="49">
-        <v>1</v>
-      </c>
-      <c r="E4" s="21">
+      <c r="F4" s="21">
         <v>0.78</v>
       </c>
-      <c r="F4" s="21">
+      <c r="G4" s="21">
         <v>0.47499999999999998</v>
       </c>
-      <c r="G4" s="22">
+      <c r="H4" s="22">
         <v>0.75</v>
       </c>
-      <c r="H4" s="22">
+      <c r="I4" s="22">
         <v>0</v>
       </c>
-      <c r="I4" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="6">
+      <c r="J4" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M4" s="6">
         <v>15</v>
       </c>
-      <c r="M4" s="22">
+      <c r="N4" s="22">
         <f t="shared" si="0"/>
         <v>1.8238704957353082</v>
       </c>
-      <c r="N4" s="79">
+      <c r="O4" s="72">
         <v>3</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="P4" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>80</v>
+    <row r="5" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="82">
+        <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="49">
-        <v>1</v>
-      </c>
-      <c r="E5" s="21">
+      <c r="F5" s="21">
         <v>1.33</v>
       </c>
-      <c r="F5" s="21">
+      <c r="G5" s="21">
         <v>0.47499999999999998</v>
       </c>
-      <c r="G5" s="22">
-        <v>1</v>
-      </c>
       <c r="H5" s="22">
+        <v>1</v>
+      </c>
+      <c r="I5" s="22">
         <v>0</v>
       </c>
-      <c r="I5" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="6">
+      <c r="J5" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" s="6">
         <v>30</v>
       </c>
-      <c r="M5" s="22">
+      <c r="N5" s="22">
         <f t="shared" si="0"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="N5" s="79">
+      <c r="O5" s="72">
         <v>4</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="P5" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>81</v>
+    <row r="6" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="82">
+        <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="50">
-        <v>1</v>
-      </c>
-      <c r="E6" s="19">
+      <c r="F6" s="19">
         <v>0.35</v>
       </c>
-      <c r="F6" s="19">
+      <c r="G6" s="19">
         <v>0.4</v>
       </c>
-      <c r="G6" s="20">
+      <c r="H6" s="20">
         <v>0.1</v>
       </c>
-      <c r="H6" s="23">
+      <c r="I6" s="23">
         <v>0</v>
       </c>
-      <c r="I6" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="4">
+      <c r="J6" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M6" s="4">
         <v>5</v>
       </c>
-      <c r="M6" s="20">
+      <c r="N6" s="20">
         <f t="shared" si="0"/>
         <v>0.30397841595588471</v>
       </c>
-      <c r="N6" s="78">
+      <c r="O6" s="71">
         <v>0.5</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="P6" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>81</v>
+    <row r="7" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="82">
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="49">
-        <v>1</v>
-      </c>
-      <c r="E7" s="21">
+      <c r="F7" s="21">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F7" s="21">
+      <c r="G7" s="21">
         <v>0.5</v>
       </c>
-      <c r="G7" s="22">
+      <c r="H7" s="22">
         <v>0.3</v>
       </c>
-      <c r="H7" s="22">
+      <c r="I7" s="22">
         <v>0</v>
       </c>
-      <c r="I7" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" s="6">
+      <c r="J7" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M7" s="6">
         <v>17</v>
       </c>
-      <c r="M7" s="22">
+      <c r="N7" s="22">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="N7" s="79">
-        <v>1</v>
-      </c>
-      <c r="O7" s="12" t="s">
+      <c r="O7" s="72">
+        <v>1</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>81</v>
+    <row r="8" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="82">
+        <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="49">
-        <v>1</v>
-      </c>
-      <c r="E8" s="21">
+      <c r="F8" s="21">
         <v>0.75</v>
       </c>
-      <c r="F8" s="21">
+      <c r="G8" s="21">
         <v>0.4</v>
       </c>
-      <c r="G8" s="22">
+      <c r="H8" s="22">
         <v>0.75</v>
       </c>
-      <c r="H8" s="22">
+      <c r="I8" s="22">
         <v>0</v>
       </c>
-      <c r="I8" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K8" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" s="6">
+      <c r="J8" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" s="6">
         <v>37</v>
       </c>
-      <c r="M8" s="22">
+      <c r="N8" s="22">
         <f t="shared" si="0"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="N8" s="79">
+      <c r="O8" s="72">
         <v>2</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="P8" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>81</v>
+    <row r="9" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="82">
+        <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="49">
-        <v>1</v>
-      </c>
-      <c r="E9" s="21">
-        <v>1</v>
-      </c>
       <c r="F9" s="21">
+        <v>1</v>
+      </c>
+      <c r="G9" s="21">
         <v>0.4</v>
       </c>
-      <c r="G9" s="22">
-        <v>1</v>
-      </c>
       <c r="H9" s="22">
+        <v>1</v>
+      </c>
+      <c r="I9" s="22">
         <v>0</v>
       </c>
-      <c r="I9" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" s="17">
+      <c r="J9" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L9" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9" s="17">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="M9" s="22">
+      <c r="N9" s="22">
         <f t="shared" si="0"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="N9" s="79">
+      <c r="O9" s="72">
         <v>4</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="P9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>83</v>
+    <row r="10" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="82">
+        <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="50">
-        <v>1</v>
-      </c>
-      <c r="E10" s="19">
+      <c r="F10" s="19">
         <v>0.75</v>
       </c>
-      <c r="F10" s="19">
+      <c r="G10" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G10" s="20">
+      <c r="H10" s="20">
         <v>0.03</v>
       </c>
-      <c r="H10" s="23">
+      <c r="I10" s="23">
         <v>0</v>
       </c>
-      <c r="I10" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" s="4">
+      <c r="J10" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L10" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="4">
         <v>3</v>
       </c>
-      <c r="M10" s="20">
+      <c r="N10" s="20">
         <f t="shared" si="0"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="N10" s="78">
-        <v>1</v>
-      </c>
-      <c r="O10" s="11" t="s">
+      <c r="O10" s="71">
+        <v>1</v>
+      </c>
+      <c r="P10" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>83</v>
+    <row r="11" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="82">
+        <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="49">
-        <v>1</v>
-      </c>
-      <c r="E11" s="21">
-        <v>1</v>
-      </c>
       <c r="F11" s="21">
+        <v>1</v>
+      </c>
+      <c r="G11" s="21">
         <v>0.3</v>
       </c>
-      <c r="G11" s="22">
+      <c r="H11" s="22">
         <v>0.15</v>
       </c>
-      <c r="H11" s="22">
+      <c r="I11" s="22">
         <v>0</v>
       </c>
-      <c r="I11" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="J11" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M11" s="6">
         <v>20</v>
       </c>
-      <c r="M11" s="22">
+      <c r="N11" s="22">
         <f t="shared" si="0"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="N11" s="79">
+      <c r="O11" s="72">
         <v>2</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="P11" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>83</v>
+    <row r="12" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="82">
+        <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="49">
-        <v>1</v>
-      </c>
-      <c r="E12" s="21">
+      <c r="F12" s="21">
         <v>1.33</v>
       </c>
-      <c r="F12" s="21">
+      <c r="G12" s="21">
         <v>0.34</v>
       </c>
-      <c r="G12" s="22">
+      <c r="H12" s="22">
         <v>0.4</v>
       </c>
-      <c r="H12" s="22">
+      <c r="I12" s="22">
         <v>0</v>
       </c>
-      <c r="I12" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" s="6">
+      <c r="J12" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L12" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M12" s="6">
         <v>60</v>
       </c>
-      <c r="M12" s="22">
+      <c r="N12" s="22">
         <f t="shared" si="0"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="N12" s="79">
+      <c r="O12" s="72">
         <v>4</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="P12" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>83</v>
+    <row r="13" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="82">
+        <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="49">
-        <v>1</v>
-      </c>
-      <c r="E13" s="21">
+      <c r="F13" s="21">
         <v>1.55</v>
       </c>
-      <c r="F13" s="21">
+      <c r="G13" s="21">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G13" s="22">
+      <c r="H13" s="22">
         <v>1.2</v>
       </c>
-      <c r="H13" s="22">
+      <c r="I13" s="22">
         <v>0</v>
       </c>
-      <c r="I13" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K13" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L13" s="17">
+      <c r="J13" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" s="17">
         <f>24*30/7</f>
         <v>102.85714285714286</v>
       </c>
-      <c r="M13" s="22">
+      <c r="N13" s="22">
         <f t="shared" si="0"/>
         <v>4.8636546552941553</v>
       </c>
-      <c r="N13" s="79">
+      <c r="O13" s="72">
         <v>8</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="P13" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>82</v>
+    <row r="14" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="82">
+        <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="50">
-        <v>1</v>
-      </c>
-      <c r="E14" s="19">
+      <c r="F14" s="19">
         <v>0.47500000000000003</v>
       </c>
-      <c r="F14" s="19">
+      <c r="G14" s="19">
         <v>0.25</v>
       </c>
-      <c r="G14" s="20">
+      <c r="H14" s="20">
         <v>0.06</v>
       </c>
-      <c r="H14" s="20">
-        <v>1</v>
-      </c>
-      <c r="I14" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="K14" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="L14" s="74">
+      <c r="I14" s="20">
+        <v>1</v>
+      </c>
+      <c r="J14" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" s="67">
         <v>5</v>
       </c>
-      <c r="M14" s="80">
-        <f t="shared" ref="M14:M17" si="1">N14/NORMINV(0.95,0,1)</f>
+      <c r="N14" s="73">
+        <f t="shared" ref="N14:N17" si="1">O14/NORMINV(0.95,0,1)</f>
         <v>0.30397841595588471</v>
       </c>
-      <c r="N14" s="81">
+      <c r="O14" s="74">
         <v>0.5</v>
       </c>
-      <c r="O14" s="11"/>
-    </row>
-    <row r="15" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>82</v>
+      <c r="P14" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="82">
+        <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="49">
-        <v>1</v>
-      </c>
-      <c r="E15" s="21">
+      <c r="F15" s="21">
         <v>0.61499999999999999</v>
       </c>
-      <c r="F15" s="21">
+      <c r="G15" s="21">
         <v>0.33</v>
       </c>
-      <c r="G15" s="22">
+      <c r="H15" s="22">
         <v>0.3</v>
       </c>
-      <c r="H15" s="22">
-        <v>1</v>
-      </c>
-      <c r="I15" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K15" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L15" s="75">
+      <c r="I15" s="22">
+        <v>1</v>
+      </c>
+      <c r="J15" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L15" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M15" s="68">
         <v>17</v>
       </c>
-      <c r="M15" s="82">
+      <c r="N15" s="75">
         <f t="shared" si="1"/>
         <v>0.60795683191176941</v>
       </c>
-      <c r="N15" s="83">
-        <v>1</v>
-      </c>
-      <c r="O15" s="12"/>
-    </row>
-    <row r="16" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>82</v>
+      <c r="O15" s="76">
+        <v>1</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="82">
+        <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="49">
-        <v>1</v>
-      </c>
-      <c r="E16" s="21">
+      <c r="F16" s="21">
         <v>0.77</v>
       </c>
-      <c r="F16" s="21">
+      <c r="G16" s="21">
         <v>0.4</v>
       </c>
-      <c r="G16" s="22">
+      <c r="H16" s="22">
         <v>0.75</v>
       </c>
-      <c r="H16" s="22">
+      <c r="I16" s="22">
         <v>0</v>
       </c>
-      <c r="I16" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="J16" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="K16" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" s="75">
+      <c r="J16" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L16" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M16" s="68">
         <v>37</v>
       </c>
-      <c r="M16" s="82">
+      <c r="N16" s="75">
         <f t="shared" si="1"/>
         <v>1.2159136638235388</v>
       </c>
-      <c r="N16" s="83">
+      <c r="O16" s="76">
         <v>2</v>
       </c>
-      <c r="O16" s="12"/>
-    </row>
-    <row r="17" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>82</v>
+      <c r="P16" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="82">
+        <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="51">
-        <v>1</v>
-      </c>
-      <c r="E17" s="24">
-        <v>1</v>
-      </c>
       <c r="F17" s="24">
+        <v>1</v>
+      </c>
+      <c r="G17" s="24">
         <v>0.4</v>
       </c>
-      <c r="G17" s="25">
-        <v>1</v>
-      </c>
       <c r="H17" s="25">
+        <v>1</v>
+      </c>
+      <c r="I17" s="25">
         <v>0</v>
       </c>
-      <c r="I17" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="J17" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="K17" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="L17" s="76">
+      <c r="J17" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17" s="69">
         <f>18*30/7</f>
         <v>77.142857142857139</v>
       </c>
-      <c r="M17" s="82">
+      <c r="N17" s="75">
         <f t="shared" si="1"/>
         <v>2.4318273276470777</v>
       </c>
-      <c r="N17" s="83">
+      <c r="O17" s="76">
         <v>4</v>
       </c>
-      <c r="O17" s="13"/>
-    </row>
-    <row r="18" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="P17" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="82">
+        <v>17</v>
+      </c>
+      <c r="B18" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="C18" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="D18" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="59">
-        <v>1</v>
-      </c>
-      <c r="E18" s="60">
+      <c r="F18" s="55">
         <v>10</v>
       </c>
-      <c r="F18" s="60">
+      <c r="G18" s="55">
         <v>0.01</v>
       </c>
-      <c r="G18" s="61">
+      <c r="H18" s="56">
         <v>0.01</v>
       </c>
-      <c r="H18" s="61">
-        <v>1</v>
-      </c>
-      <c r="I18" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="K18" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="L18" s="62">
-        <v>1</v>
-      </c>
-      <c r="M18" s="61">
-        <f t="shared" ref="M18:M25" si="2">N18/NORMINV(0.95,0,1)</f>
+      <c r="I18" s="56">
+        <v>1</v>
+      </c>
+      <c r="J18" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M18" s="57">
+        <v>1</v>
+      </c>
+      <c r="N18" s="56">
+        <f t="shared" ref="N18:N25" si="2">O18/NORMINV(0.95,0,1)</f>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="N18" s="84">
+      <c r="O18" s="77">
         <v>0.1</v>
       </c>
-      <c r="O18" s="11"/>
-    </row>
-    <row r="19" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="s">
+      <c r="P18" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="82">
+        <v>18</v>
+      </c>
+      <c r="B19" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="C19" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="63" t="s">
+      <c r="D19" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="64">
-        <v>1</v>
-      </c>
-      <c r="E19" s="65">
+      <c r="F19" s="59">
         <v>10</v>
       </c>
-      <c r="F19" s="65">
+      <c r="G19" s="59">
         <v>0.01</v>
       </c>
-      <c r="G19" s="66">
+      <c r="H19" s="60">
         <v>0.01</v>
       </c>
-      <c r="H19" s="66">
-        <v>1</v>
-      </c>
-      <c r="I19" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="J19" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="K19" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="L19" s="67">
-        <v>1</v>
-      </c>
-      <c r="M19" s="66">
+      <c r="I19" s="60">
+        <v>1</v>
+      </c>
+      <c r="J19" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L19" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M19" s="61">
+        <v>1</v>
+      </c>
+      <c r="N19" s="60">
         <f t="shared" si="2"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="N19" s="85">
+      <c r="O19" s="78">
         <v>0.1</v>
       </c>
-      <c r="O19" s="12"/>
-    </row>
-    <row r="20" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="63" t="s">
+      <c r="P19" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="82">
+        <v>19</v>
+      </c>
+      <c r="B20" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="C20" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="63" t="s">
+      <c r="D20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="64">
-        <v>1</v>
-      </c>
-      <c r="E20" s="65">
+      <c r="F20" s="59">
         <v>10</v>
       </c>
-      <c r="F20" s="65">
+      <c r="G20" s="59">
         <v>0.01</v>
       </c>
-      <c r="G20" s="66">
+      <c r="H20" s="60">
         <v>0.01</v>
       </c>
-      <c r="H20" s="66">
-        <v>1</v>
-      </c>
-      <c r="I20" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="J20" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="K20" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="L20" s="67">
-        <v>1</v>
-      </c>
-      <c r="M20" s="66">
+      <c r="I20" s="60">
+        <v>1</v>
+      </c>
+      <c r="J20" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="K20" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M20" s="61">
+        <v>1</v>
+      </c>
+      <c r="N20" s="60">
         <f t="shared" si="2"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="N20" s="85">
+      <c r="O20" s="78">
         <v>0.1</v>
       </c>
-      <c r="O20" s="12"/>
-    </row>
-    <row r="21" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="68" t="s">
+      <c r="P20" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="82">
+        <v>20</v>
+      </c>
+      <c r="B21" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="C21" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="68" t="s">
+      <c r="D21" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="69">
-        <v>1</v>
-      </c>
-      <c r="E21" s="70">
+      <c r="F21" s="63">
         <v>10</v>
       </c>
-      <c r="F21" s="70">
+      <c r="G21" s="63">
         <v>0.01</v>
       </c>
-      <c r="G21" s="71">
+      <c r="H21" s="64">
         <v>0.01</v>
       </c>
-      <c r="H21" s="71">
-        <v>1</v>
-      </c>
-      <c r="I21" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="J21" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="K21" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="L21" s="72">
-        <v>1</v>
-      </c>
-      <c r="M21" s="71">
+      <c r="I21" s="64">
+        <v>1</v>
+      </c>
+      <c r="J21" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="K21" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L21" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M21" s="65">
+        <v>1</v>
+      </c>
+      <c r="N21" s="64">
         <f t="shared" si="2"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="N21" s="86">
+      <c r="O21" s="79">
         <v>0.1</v>
       </c>
-      <c r="O21" s="13"/>
-    </row>
-    <row r="22" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="58" t="s">
+      <c r="P21" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="82">
+        <v>21</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="D22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="59">
-        <v>1</v>
-      </c>
-      <c r="E22" s="60">
+      <c r="F22" s="55">
         <v>10</v>
       </c>
-      <c r="F22" s="60">
+      <c r="G22" s="55">
         <v>0.01</v>
       </c>
-      <c r="G22" s="61">
+      <c r="H22" s="56">
         <v>0.01</v>
       </c>
-      <c r="H22" s="61">
-        <v>1</v>
-      </c>
-      <c r="I22" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="K22" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="L22" s="62">
-        <v>1</v>
-      </c>
-      <c r="M22" s="61">
+      <c r="I22" s="56">
+        <v>1</v>
+      </c>
+      <c r="J22" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="K22" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L22" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M22" s="57">
+        <v>1</v>
+      </c>
+      <c r="N22" s="56">
         <f t="shared" si="2"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="N22" s="84">
+      <c r="O22" s="77">
         <v>0.1</v>
       </c>
-      <c r="O22" s="11"/>
-    </row>
-    <row r="23" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="63" t="s">
+      <c r="P22" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="82">
+        <v>22</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="D23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="64">
-        <v>1</v>
-      </c>
-      <c r="E23" s="65">
+      <c r="F23" s="59">
         <v>10</v>
       </c>
-      <c r="F23" s="65">
+      <c r="G23" s="59">
         <v>0.01</v>
       </c>
-      <c r="G23" s="66">
+      <c r="H23" s="60">
         <v>0.01</v>
       </c>
-      <c r="H23" s="66">
-        <v>1</v>
-      </c>
-      <c r="I23" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="J23" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="K23" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="L23" s="67">
-        <v>1</v>
-      </c>
-      <c r="M23" s="66">
+      <c r="I23" s="60">
+        <v>1</v>
+      </c>
+      <c r="J23" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L23" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M23" s="61">
+        <v>1</v>
+      </c>
+      <c r="N23" s="60">
         <f t="shared" si="2"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="N23" s="85">
+      <c r="O23" s="78">
         <v>0.1</v>
       </c>
-      <c r="O23" s="12"/>
-    </row>
-    <row r="24" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="63" t="s">
+      <c r="P23" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="82">
+        <v>23</v>
+      </c>
+      <c r="B24" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="63" t="s">
+      <c r="D24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="64">
-        <v>1</v>
-      </c>
-      <c r="E24" s="65">
+      <c r="F24" s="59">
         <v>10</v>
       </c>
-      <c r="F24" s="65">
+      <c r="G24" s="59">
         <v>0.01</v>
       </c>
-      <c r="G24" s="66">
+      <c r="H24" s="60">
         <v>0.01</v>
       </c>
-      <c r="H24" s="66">
-        <v>1</v>
-      </c>
-      <c r="I24" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="J24" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="K24" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="L24" s="67">
-        <v>1</v>
-      </c>
-      <c r="M24" s="66">
+      <c r="I24" s="60">
+        <v>1</v>
+      </c>
+      <c r="J24" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L24" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M24" s="61">
+        <v>1</v>
+      </c>
+      <c r="N24" s="60">
         <f t="shared" si="2"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="N24" s="85">
+      <c r="O24" s="78">
         <v>0.1</v>
       </c>
-      <c r="O24" s="12"/>
-    </row>
-    <row r="25" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="68" t="s">
+      <c r="P24" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="82">
+        <v>24</v>
+      </c>
+      <c r="B25" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="68" t="s">
+      <c r="D25" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="69">
-        <v>1</v>
-      </c>
-      <c r="E25" s="70">
+      <c r="F25" s="63">
         <v>10</v>
       </c>
-      <c r="F25" s="70">
+      <c r="G25" s="63">
         <v>0.01</v>
       </c>
-      <c r="G25" s="71">
+      <c r="H25" s="64">
         <v>0.01</v>
       </c>
-      <c r="H25" s="71">
-        <v>1</v>
-      </c>
-      <c r="I25" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="J25" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="K25" s="71" t="s">
-        <v>55</v>
-      </c>
-      <c r="L25" s="72">
-        <v>1</v>
-      </c>
-      <c r="M25" s="71">
+      <c r="I25" s="64">
+        <v>1</v>
+      </c>
+      <c r="J25" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="K25" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="L25" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="M25" s="65">
+        <v>1</v>
+      </c>
+      <c r="N25" s="64">
         <f t="shared" si="2"/>
         <v>6.0795683191176939E-2</v>
       </c>
-      <c r="N25" s="86">
+      <c r="O25" s="79">
         <v>0.1</v>
       </c>
-      <c r="O25" s="13"/>
+      <c r="P25" s="11" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A5:O68">
-    <sortCondition ref="A133:A196"/>
+  <sortState ref="B5:P68">
     <sortCondition ref="B133:B196"/>
+    <sortCondition ref="C133:C196"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3953,12 +4049,12 @@
         <v>5</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>16</v>
@@ -3969,7 +4065,7 @@
     </row>
     <row r="3" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>17</v>
@@ -3980,7 +4076,7 @@
     </row>
     <row r="4" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>18</v>
@@ -3991,7 +4087,7 @@
     </row>
     <row r="5" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>19</v>
@@ -4002,7 +4098,7 @@
     </row>
     <row r="6" spans="1:3" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>16</v>
@@ -4013,7 +4109,7 @@
     </row>
     <row r="7" spans="1:3" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>17</v>
@@ -4024,7 +4120,7 @@
     </row>
     <row r="8" spans="1:3" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>18</v>
@@ -4035,7 +4131,7 @@
     </row>
     <row r="9" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>19</v>
@@ -4046,7 +4142,7 @@
     </row>
     <row r="10" spans="1:3" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>16</v>
@@ -4057,7 +4153,7 @@
     </row>
     <row r="11" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>17</v>
@@ -4068,7 +4164,7 @@
     </row>
     <row r="12" spans="1:3" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>18</v>
@@ -4079,7 +4175,7 @@
     </row>
     <row r="13" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>19</v>
@@ -4090,7 +4186,7 @@
     </row>
     <row r="14" spans="1:3" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>16</v>
@@ -4101,7 +4197,7 @@
     </row>
     <row r="15" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>17</v>
@@ -4112,7 +4208,7 @@
     </row>
     <row r="16" spans="1:3" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>18</v>
@@ -4123,7 +4219,7 @@
     </row>
     <row r="17" spans="1:3" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>19</v>
@@ -4133,91 +4229,91 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="54" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="58" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="58" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="68" t="s">
+      <c r="A21" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="62" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="58" t="s">
+      <c r="A22" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="54" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="63" t="s">
+      <c r="A23" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="58" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="63" t="s">
+      <c r="A24" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="58" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="68" t="s">
+      <c r="A25" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="62" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>